<commit_message>
correlations based on spitzemapko
</commit_message>
<xml_diff>
--- a/GSEA_like_analysis/enrichments_by_quadrant_of_GAP_GEF_rank_correlation_of_library_genes_table_formatted.xlsx
+++ b/GSEA_like_analysis/enrichments_by_quadrant_of_GAP_GEF_rank_correlation_of_library_genes_table_formatted.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16340" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t>TRANSMEMBRANE TRANSPORT</t>
   </si>
   <si>
-    <t>TRNA PROCESSING</t>
-  </si>
-  <si>
     <t>HANNES CHROMATIN REMODELING</t>
   </si>
   <si>
@@ -96,7 +93,10 @@
     <t>SIGNAL TRANSDUCER ACTIVITY</t>
   </si>
   <si>
-    <t>Gene set</t>
+    <t>gene_set</t>
+  </si>
+  <si>
+    <t>tRNA PROCESSING</t>
   </si>
 </sst>
 </file>
@@ -148,8 +148,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -166,16 +178,31 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="20">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -190,6 +217,9 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -203,6 +233,9 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -214,6 +247,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -234,48 +270,48 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C2" totalsRowShown="0" headerRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C2" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A1:C2"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Gene set" dataDxfId="15"/>
-    <tableColumn id="2" name="FDR" dataDxfId="14"/>
-    <tableColumn id="3" name="quadrant" dataDxfId="13"/>
+    <tableColumn id="1" name="gene_set" dataDxfId="19"/>
+    <tableColumn id="2" name="FDR" dataDxfId="18"/>
+    <tableColumn id="3" name="quadrant" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A5:C13" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A5:C13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A4:C12" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A4:C12"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Gene set" dataDxfId="11"/>
-    <tableColumn id="2" name="FDR" dataDxfId="10"/>
-    <tableColumn id="3" name="quadrant" dataDxfId="9"/>
+    <tableColumn id="1" name="gene_set" dataDxfId="14"/>
+    <tableColumn id="2" name="FDR" dataDxfId="13"/>
+    <tableColumn id="3" name="quadrant" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table134" displayName="Table134" ref="A15:C19" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A15:C19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A14:C18" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A14:C18"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Gene set" dataDxfId="7"/>
-    <tableColumn id="2" name="FDR" dataDxfId="6"/>
-    <tableColumn id="3" name="quadrant" dataDxfId="5"/>
+    <tableColumn id="1" name="gene_set" dataDxfId="9"/>
+    <tableColumn id="2" name="FDR" dataDxfId="8"/>
+    <tableColumn id="3" name="quadrant" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table135" displayName="Table135" ref="A22:C28" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A22:C28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A20:C26" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="A20:C26"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Gene set" dataDxfId="3"/>
-    <tableColumn id="2" name="FDR" dataDxfId="2"/>
-    <tableColumn id="3" name="quadrant" dataDxfId="1"/>
+    <tableColumn id="1" name="gene_set" dataDxfId="4"/>
+    <tableColumn id="2" name="FDR" dataDxfId="3"/>
+    <tableColumn id="3" name="quadrant" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -603,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -618,7 +654,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -638,23 +674,39 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="B5" s="2">
+        <v>8.234033E-3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2">
-        <v>4.3658026000000003E-2</v>
+        <v>1.5429604E-2</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>5</v>
@@ -662,10 +714,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B7" s="2">
-        <v>7.9770369999999993E-2</v>
+        <v>3.3515113999999999E-2</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
@@ -673,10 +725,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>4.6958703999999997E-2</v>
+        <v>3.4052324000000002E-2</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
@@ -684,10 +736,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2">
-        <v>3.4052324000000002E-2</v>
+        <v>3.8566977000000002E-2</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>5</v>
@@ -695,10 +747,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B10" s="2">
-        <v>3.8566977000000002E-2</v>
+        <v>4.3658026000000003E-2</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>5</v>
@@ -706,10 +758,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B11" s="2">
-        <v>1.5429604E-2</v>
+        <v>4.6958703999999997E-2</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>5</v>
@@ -717,57 +769,62 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B12" s="2">
-        <v>8.234033E-3</v>
+        <v>7.9770369999999993E-2</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2">
-        <v>3.3515113999999999E-2</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>5</v>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1.0422710999999999E-2</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1.8106800999999999E-2</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B16" s="2">
-        <v>1.0422710999999999E-2</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="2">
         <v>2.0845422999999998E-2</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -775,43 +832,59 @@
         <v>16</v>
       </c>
       <c r="B18" s="2">
-        <v>1.8106800999999999E-2</v>
+        <v>5.0617676E-2</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="2">
-        <v>5.0617676E-2</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>14</v>
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2">
+        <v>6.7043550000000004E-3</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="B22" s="2">
+        <v>3.8070899999999998E-2</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2">
+        <v>4.6473590000000002E-2</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B23" s="2">
-        <v>3.8070899999999998E-2</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -819,10 +892,10 @@
         <v>20</v>
       </c>
       <c r="B24" s="2">
-        <v>6.7043550000000004E-3</v>
+        <v>5.9057508000000002E-2</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -830,43 +903,21 @@
         <v>21</v>
       </c>
       <c r="B25" s="2">
-        <v>5.9057508000000002E-2</v>
+        <v>6.5809060000000003E-2</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B26" s="2">
-        <v>6.5809060000000003E-2</v>
+        <v>7.8722379999999995E-2</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" s="2">
-        <v>4.6473590000000002E-2</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" s="2">
-        <v>7.8722379999999995E-2</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>